<commit_message>
poitou charente completed with towns json and characters json
</commit_message>
<xml_diff>
--- a/data/outputs/deux-sevres/deux-sevres.xlsx
+++ b/data/outputs/deux-sevres/deux-sevres.xlsx
@@ -512,7 +512,7 @@
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Québec</t>
+          <t>21-06-1763</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -544,7 +544,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Inconnu</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -572,7 +572,7 @@
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Hôtel-Dieu de Québec</t>
+          <t>Québec</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -683,12 +683,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Saint-Pierre</t>
+          <t>Église Saint-Pierre</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Saint-Jean, Île d'Orléans (Qc)</t>
+          <t>Saint-Jean, Île d’Orléans (Qc)</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Saint-André</t>
+          <t>Paroisse Saint-André</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -901,7 +901,11 @@
           <t>BAREAU dit Bréliau, Jean. Né en 1651. Fils de Jean Bareau et de Françoise Cellier. Marié à Jeanne Cusson, à Cap-de-la-Madeleine (Qc), le 09-11-1679. Quatre enfants. Décédé à Laprairie (Qc), le 04-09-1690, tué par les Iroquois. Cité à Laprairie (Qc), le 17-08-1673. (IFGH)</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Inconnu</t>
+        </is>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>Laprairie (Qc)</t>
@@ -1047,7 +1051,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>prieuré Saint-Maixent de Verrines</t>
+          <t>Prieuré Saint-Maixent de Verrines</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1080,7 +1084,7 @@
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Québec</t>
+          <t>Hôtel-Dieu de Québec</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1140,7 +1144,7 @@
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>En 1758</t>
+          <t>1758</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1287,7 +1291,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Non spécifié</t>
+          <t>Saint-André</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1319,7 +1323,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Saint-Jean</t>
+          <t>Paroisse Saint-Jean</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1351,12 +1355,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Pas spécifié</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Québec</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1409,14 +1413,10 @@
           <t>BILODEAU, Jérôme. Né vers 1636. Fils de Jérôme Bilodeau et de Marie Gandillard. Marié à Jeanne Ripoche, à Québec, le 04-02-1664. Décédé en France, après 1670. Engagé chez le notaire Cherbonnier, à La Rochelle (Fr.), pour la Nouvelle-France, le 15-03-1657. (FO)</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
+      <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Inconnu</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1521,11 +1521,7 @@
           <t>BLANCHET dit Laforest, Pierre. Meunier. Né en 1643. Fils de René Blanchet et de Marie-Jeanne Marier. Marié à Marie-Françoise Harel, à Champlain (Qc), le 04-07-1696. Six enfants. Inhumé à Trois-Rivières (Qc), le 03-12-1708. (IFGH)</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Non spécifié</t>
-        </is>
-      </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
           <t>Trois-Rivières (Qc)</t>
@@ -1587,7 +1583,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>La Rochelle (France)</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1803,7 +1799,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Inconnu (entre 1666 et 1676)</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1835,7 +1831,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Église Saint-Germain</t>
+          <t>Saint-Germain</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1897,16 +1893,8 @@
           <t>BOURDEAU dit Leroux, Isaac. Fils d’Abraham Bourdeau et de Catherine Rousseau. Marié à Marie ou Marie-Françoise Courault, à Chambly (Qc), le 20-01-1718. Quatre enfants. (IFGH)</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Non spécifié</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Chambly (Qc)</t>
-        </is>
-      </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr"/>
       <c r="F49" t="inlineStr">
         <is>
           <t>SAINT-COUTANT (79120)</t>
@@ -2013,11 +2001,7 @@
           <t>BREUILLARD ou BREUILLAC dit Laroche, Amable. Né vers 1652. Fils de Daniel Breuillac et de Jeanne Courtin. Marié à Marie Lafond, à Batiscan (Qc), le 13-02-1687. Neuf enfants. Décédé à Varennes (Qc), le 10-04-1736. Mentionné en Nouvelle-France, en 1687. (FO-IFGH)</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
+      <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
           <t>Varennes (Qc)</t>
@@ -2107,7 +2091,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Notre-Dame</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2137,8 +2121,16 @@
           <t>BUREAU, Isaac. Né vers 1733. Fils d’Isaac Bureau et de Marie Modet. Marié à Marie-Angélique Girard, à Montréal (Qc), le 10-01-1757. (IFGH)</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Non spécifié</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Montréal (Qc)</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr">
         <is>
           <t>MAUZÉ-SUR-LE-MIGNON (79210)</t>
@@ -2161,11 +2153,7 @@
           <t>CADET, Michel. Boucher. Né vers 1665. Fils de Michel Cadet et d’Élisabeth Fièbvre. Marié à 1) Marie Constantin, à Québec, le 25-01-1694. Six enfants. 2) Geneviève Gauthier, à Québec, le 26-04-1703. Quatre enfants. Décédé à Québec, en 1708. Il abjure sa religion protestante, à Niort, le 21-08-1685. Première mention, à l’Hôtel-Dieu de Québec, le 05-06-1690. (IFGH)</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
+      <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
           <t>Québec</t>
@@ -2279,7 +2267,7 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Eglise Saint-Porchaire</t>
+          <t>Saint-Porchaire</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -2448,7 +2436,7 @@
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
-          <t>L’Ancienne-Lorette (Qc)</t>
+          <t>L'Ancienne-Lorette (Qc)</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -2588,7 +2576,7 @@
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Québec</t>
+          <t>Hôtel-Dieu de Québec</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -2729,7 +2717,11 @@
           <t>DEQUAIN, Anne. Fille du Roy. Née vers 1645. Fille de Fleurimon Degain et d’Henriette Demeuis. Mariée à François Lareau, à Québec, le 28-10-1669. Décédée à la Petite-Rivière-Saint-François (Qc), en 1734. (ILMPC)</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr"/>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Non spécifié</t>
+        </is>
+      </c>
       <c r="E78" t="inlineStr">
         <is>
           <t>Petite-Rivière-Saint-François (Qc)</t>
@@ -2853,11 +2845,7 @@
           <t>DROUARD, Marie-Anne. Fille de Fleurant Drouard et de Jeanne Mathieu. Mariée à Jean-François Hazeur, à La Rochelle (Fr.), le 01-02-1672. Un enfant. Décédé à Québec, le 08-12-1690. (IFGH)</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>Non spécifié</t>
-        </is>
-      </c>
+      <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr">
         <is>
           <t>Québec</t>
@@ -2885,16 +2873,8 @@
           <t>DUPONT dit Vadeboncoeur, Jacques. Sergent. Fils de Jacques Dupont et de Jeanne Fouladou. Marié à Marie-Anne Trotier, à Montréal (Qc), le 22-11-1735. (IFGH)</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>Pas spécifié</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>Pas spécifié</t>
-        </is>
-      </c>
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr">
         <is>
           <t>BRIOUX-SUR-BOUTONNE (79170)</t>
@@ -2976,7 +2956,7 @@
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Nouvelle-France (env. 1730)</t>
+          <t>Nouvelle-France</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -3173,8 +3153,16 @@
           <t>FOURNIER dit Brisefer, Pierre. Fils de Pierre Fournier et de Marguerite-Hélène Métayer. Marié à Marie-Louise Lienard, à Québec, le 29-09-1749. (IFGH)</t>
         </is>
       </c>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Non spécifié</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Québec</t>
+        </is>
+      </c>
       <c r="F93" t="inlineStr">
         <is>
           <t>NIORT (79000)</t>
@@ -3279,7 +3267,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Notre-Dame</t>
+          <t>Paroisse Notre-Dame</t>
         </is>
       </c>
       <c r="E97" t="inlineStr"/>
@@ -3331,7 +3319,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Non spécifié</t>
+          <t>Données introuvables</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -3368,7 +3356,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Inconnu</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -3727,10 +3715,14 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Paroisse Saint-Liguaire</t>
-        </is>
-      </c>
-      <c r="E112" t="inlineStr"/>
+          <t>Saint-Liguaire</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Non spécifié</t>
+        </is>
+      </c>
       <c r="F112" t="inlineStr">
         <is>
           <t>NIORT (79000)</t>
@@ -3760,7 +3752,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Non spécifié</t>
+          <t>Not Specified</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -3787,7 +3779,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Sainte-Marie-Madeleine</t>
+          <t>Paroisse Sainte-Marie-Madeleine</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -3879,12 +3871,12 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Saint-André</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Québec, l'Hôtel-Dieu de Québec</t>
+          <t>Québec</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -4040,7 +4032,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Entre 1703 et 1706</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -4157,16 +4149,8 @@
           <t>LA CROSSE, Mathurine. Née en 1635. Fille de Jean La Crosse et de Nolette de Veau. Elle est enceinte et engagée par François Péron, à La Rochelle (Fr.) et s’embarque sur le navire « le Taureau ». Première mention en Nouvelle-France, en 1658. Renvoyée par le gouverneur Voyer d’Argenson. Mariée à Pierre Nobileau, à La Rochelle (Fr.), dans l’église du Couvent d’oratoriens Sainte-Marguerite « L’Oratoire », en 1666. (ILMPC)</t>
         </is>
       </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t>Non spécifié</t>
-        </is>
-      </c>
-      <c r="E126" t="inlineStr">
-        <is>
-          <t>La Rochelle, France</t>
-        </is>
-      </c>
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="inlineStr"/>
       <c r="F126" t="inlineStr">
         <is>
           <t>FORS (79230)</t>
@@ -4279,12 +4263,12 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>Inconnu</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Inconnu</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -4404,7 +4388,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Charlesbourg, Qc</t>
+          <t>Charlesbourg (Qc)</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -4462,11 +4446,7 @@
           <t>Notre-Dame</t>
         </is>
       </c>
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>Vide</t>
-        </is>
-      </c>
+      <c r="E136" t="inlineStr"/>
       <c r="F136" t="inlineStr">
         <is>
           <t>NIORT (79000)</t>
@@ -4547,12 +4527,12 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Non spécifié</t>
+          <t>temple calviniste</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Non spécifié</t>
+          <t>non spécifié</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -4659,7 +4639,7 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>Inconnu</t>
+          <t>Données introuvables</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -4722,11 +4702,7 @@
           <t>Saint-Grégoire</t>
         </is>
       </c>
-      <c r="E145" t="inlineStr">
-        <is>
-          <t>Inconnu</t>
-        </is>
-      </c>
+      <c r="E145" t="inlineStr"/>
       <c r="F145" t="inlineStr">
         <is>
           <t>AUGÉ (79400)</t>
@@ -4783,7 +4759,7 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>Paroisse Saint-Saturnin</t>
+          <t>Saint-Saturnin</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -4908,7 +4884,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Sainte-Famille, Île-d’Orléans (Qc)</t>
+          <t>Île-d’Orléans (Qc), Sainte-Famille</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -4996,7 +4972,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>Neuville (Qc)</t>
+          <t>Neuville</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -5051,12 +5027,12 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Inconnu</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Port-Lajoie, Nouveau-Brunswick</t>
+          <t>Port-Lajoie (Nouveau-Brunswick)</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -5113,7 +5089,11 @@
           <t>PERRAULT* ou PAYRAULT, Jean. Baptisé le 19-09-1731, paroisse Saint-Pierre. Fils de Jean Perrault et de Marie-Jeanne Guérineau. Marié à Marie-Anne Ménard, à Montréal (Qc), le 27-06-1752. Décédé à Chambly (Qc), le 31-12-1809. Parti en Nouvelle-France, avec ses parents, en 1743. (FO)</t>
         </is>
       </c>
-      <c r="D158" t="inlineStr"/>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Non spécifié</t>
+        </is>
+      </c>
       <c r="E158" t="inlineStr">
         <is>
           <t>Chambly (Qc)</t>
@@ -5143,7 +5123,7 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>Paroisse Saint-Pierre</t>
+          <t>Saint-Pierre</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -5175,7 +5155,7 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>Paroisse Saint-André</t>
+          <t>Saint-André</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -5244,7 +5224,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Non spécifié</t>
+          <t>Saint-Pierre, Île-d’Orléans (Qc)</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -5299,12 +5279,12 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>chapelle Notre-Dame</t>
+          <t>Notre-Dame</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Champlain (Qc)</t>
+          <t>Champlain</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -5329,16 +5309,8 @@
           <t>PATRY, André. Fils d’André Patry et de Renée Cousineau. Marié à Henriette Cartois, fille du Roy, à Québec, le 23-05-1675. Trois enfants. (FG)</t>
         </is>
       </c>
-      <c r="D165" t="inlineStr">
-        <is>
-          <t>Non spécifié</t>
-        </is>
-      </c>
-      <c r="E165" t="inlineStr">
-        <is>
-          <t>Non spécifié</t>
-        </is>
-      </c>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="inlineStr"/>
       <c r="F165" t="inlineStr">
         <is>
           <t>AIRVAULT (79600)</t>
@@ -5454,11 +5426,7 @@
         </is>
       </c>
       <c r="D169" t="inlineStr"/>
-      <c r="E169" t="inlineStr">
-        <is>
-          <t>Montréal, Qc</t>
-        </is>
-      </c>
+      <c r="E169" t="inlineStr"/>
       <c r="F169" t="inlineStr">
         <is>
           <t>MONTALEMBERT (79190)</t>
@@ -5576,7 +5544,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Saint-Joachim</t>
+          <t>Saint-Joachim (Qc)</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -5667,14 +5635,10 @@
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>Notre-Dame</t>
-        </is>
-      </c>
-      <c r="E176" t="inlineStr">
-        <is>
-          <t>Valeur introuvable ou non spécifiée</t>
-        </is>
-      </c>
+          <t>église Notre-Dame</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr"/>
       <c r="F176" t="inlineStr">
         <is>
           <t>MELLERAN (79190)</t>
@@ -5699,12 +5663,12 @@
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>Inconnu (car il a été baptisé)</t>
+          <t>Inconnu</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>Inconnu</t>
+          <t>Québec</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -5731,7 +5695,7 @@
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Paroisse Saint-André</t>
+          <t>Saint-André</t>
         </is>
       </c>
       <c r="E178" t="inlineStr"/>
@@ -5791,12 +5755,12 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Inconnu</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>Inconnu</t>
+          <t>Non spécifié</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -5823,7 +5787,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>Non spécifié</t>
+          <t>Inconnu</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
@@ -5941,10 +5905,14 @@
           <t>VEILLET, Jean. Militaire. Né en 1661, se déclare originaire de la paroisse Saint-André. Marié à Catherine Lariou, à Batiscan (Qc), le 19-11-1698. Décédé, en 1741. Il abjure sa foi protestante, en 1685, dans l’église Saint-André et traverse l’Atlantique, en 1687 au départ de La Rochelle. Soldat des troupes de la Marine, compagnie de Vaudreuil. (ILMPC)</t>
         </is>
       </c>
-      <c r="D185" t="inlineStr"/>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Inconnu</t>
+        </is>
+      </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>Batiscan (Qc)</t>
+          <t>Décès en 1741 (Lieu inconnu)</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -5971,12 +5939,12 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Né en 1604 signifie que la date de naissance est inconnue, mais elle est baptisée en ce lieu</t>
+          <t>Inconnu</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>Elle meurt en 1674</t>
+          <t>Inconnu</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">

</xml_diff>